<commit_message>
remove data ovsapp from data worksheet
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nightraven/Coding/optimization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nightraven/Coding/optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E9E8B1-5E53-C241-AD6B-2CFA62991436}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95FAB01-CB66-1341-8EF9-64841DAD2301}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="1" xr2:uid="{B2749FFB-0B73-CB4B-8F68-DFBB1FB562D1}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{B2749FFB-0B73-CB4B-8F68-DFBB1FB562D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -374,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D73ABA66-4B1B-494E-BC7F-C6433B968326}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -558,17 +558,6 @@
         <v>2.13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>3.944</v>
-      </c>
-      <c r="B17">
-        <v>3.9889999999999999</v>
-      </c>
-      <c r="C17">
-        <v>4.1289999999999996</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -576,10 +565,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7755C020-212A-EB4C-B960-D863E5D39A44}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -738,17 +727,6 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>3.911</v>
-      </c>
-      <c r="B15">
-        <v>3.823</v>
-      </c>
-      <c r="C15">
-        <v>3.8079999999999998</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -756,10 +734,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC96CE7B-1AC4-5A4B-A6D8-A2CB2A1E20C4}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C13"/>
+      <selection activeCell="A13" sqref="A13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -896,17 +874,6 @@
         <v>6.3E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>1.6060000000000001</v>
-      </c>
-      <c r="B13">
-        <v>1.74</v>
-      </c>
-      <c r="C13">
-        <v>1.149</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -914,10 +881,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E6EFE71-D863-ED46-ABC8-7D2D3F48606F}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C17"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1098,17 +1065,6 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>2.2080000000000002</v>
-      </c>
-      <c r="B17">
-        <v>2.6779999999999999</v>
-      </c>
-      <c r="C17">
-        <v>1.8879999999999999</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
remove fix bug from sorting
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nightraven/Coding/optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95FAB01-CB66-1341-8EF9-64841DAD2301}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE549A63-08FC-AB4A-A57D-F459E4F2A22B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{B2749FFB-0B73-CB4B-8F68-DFBB1FB562D1}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16320" activeTab="1" xr2:uid="{B2749FFB-0B73-CB4B-8F68-DFBB1FB562D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -376,7 +376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D73ABA66-4B1B-494E-BC7F-C6433B968326}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17:C17"/>
     </sheetView>
   </sheetViews>
@@ -565,10 +565,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7755C020-212A-EB4C-B960-D863E5D39A44}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -630,100 +630,89 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2.1999999999999999E-2</v>
+        <v>2.7090000000000001</v>
       </c>
       <c r="B6">
-        <v>3.1E-2</v>
+        <v>2.2040000000000002</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>3.3140000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2.7090000000000001</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="B7">
-        <v>2.2040000000000002</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="C7">
-        <v>3.3140000000000001</v>
+        <v>5.7000000000000002E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>5.1999999999999998E-2</v>
+        <v>0.61899999999999999</v>
       </c>
       <c r="B8">
-        <v>6.4000000000000001E-2</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="C8">
-        <v>5.7000000000000002E-2</v>
+        <v>0.61599999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>0.61899999999999999</v>
+        <v>1.0469999999999999</v>
       </c>
       <c r="B9">
-        <v>0.56999999999999995</v>
+        <v>0.93100000000000005</v>
       </c>
       <c r="C9">
-        <v>0.61599999999999999</v>
+        <v>1.016</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>1.0469999999999999</v>
+        <v>1.9E-2</v>
       </c>
       <c r="B10">
-        <v>0.93100000000000005</v>
+        <v>0.02</v>
       </c>
       <c r="C10">
-        <v>1.016</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>1.9E-2</v>
+        <v>0</v>
       </c>
       <c r="B11">
-        <v>0.02</v>
+        <v>1.4E-2</v>
       </c>
       <c r="C11">
-        <v>2.3E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>0</v>
+        <v>0.46600000000000003</v>
       </c>
       <c r="B12">
-        <v>1.4E-2</v>
+        <v>0.22800000000000001</v>
       </c>
       <c r="C12">
-        <v>1.0999999999999999E-2</v>
+        <v>0.28899999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>0.46600000000000003</v>
+        <v>0</v>
       </c>
       <c r="B13">
-        <v>0.22800000000000001</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="C13">
-        <v>0.28899999999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>0</v>
-      </c>
-      <c r="B14">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="C14">
         <v>0.01</v>
       </c>
     </row>

</xml_diff>